<commit_message>
Update lista de precios
</commit_message>
<xml_diff>
--- a/Documentos/lista de precios.xlsx
+++ b/Documentos/lista de precios.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVI\Desktop\DomoticMood\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javir\Desktop\DomoticMood\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451601CE-30AB-4A41-A8B2-ADD7B57E9E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF23DC58-8075-4E69-AFBA-AFBA59B024C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9F18A56C-43DA-4260-8C29-14670BEE72CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9F18A56C-43DA-4260-8C29-14670BEE72CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Componente</t>
   </si>
@@ -48,16 +48,50 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16Mhz</t>
+  </si>
+  <si>
+    <t>Capacitores 100nF</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Pineras Macho</t>
+  </si>
+  <si>
+    <t>Moc3020</t>
+  </si>
+  <si>
+    <t>Led EMISOR IR</t>
+  </si>
+  <si>
+    <t>Receptor IR</t>
+  </si>
+  <si>
+    <t>Triac</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Adaptador Smd Tqfp100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +106,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,12 +141,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -106,12 +186,25 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,13 +218,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{748F7310-11A2-4AF8-87BC-D283475CEFC2}" name="Tabla1" displayName="Tabla1" ref="A1:B62" totalsRowShown="0">
-  <autoFilter ref="A1:B62" xr:uid="{748F7310-11A2-4AF8-87BC-D283475CEFC2}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{748F7310-11A2-4AF8-87BC-D283475CEFC2}" name="Tabla1" displayName="Tabla1" ref="A1:D62" totalsRowShown="0">
+  <autoFilter ref="A1:D62" xr:uid="{748F7310-11A2-4AF8-87BC-D283475CEFC2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F383E9CE-B270-496D-9EE0-8052A35F587E}" name="Componente"/>
     <tableColumn id="2" xr3:uid="{D1140BC8-6868-49B0-9645-A355BA18AA13}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{3895AA80-0EC3-42EB-9779-341E3F835700}" name="Unidad"/>
+    <tableColumn id="4" xr3:uid="{A62C68D1-84C1-4C83-9BAB-33028F811657}" name="Total" dataDxfId="0">
+      <calculatedColumnFormula>PRODUCT(B2,C2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -432,112 +534,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA7C316-E20C-47BC-8E77-A036621AE5C7}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>440</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D33" si="0">PRODUCT(B2,C2)</f>
+        <v>440</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7">
+        <f>SUBTOTAL(109,B2:B61)</f>
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>1440</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>150</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>150</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>225</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>385</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="6"/>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="6"/>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="6"/>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="6"/>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="6"/>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+      <c r="D28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="6"/>
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="6"/>
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="6"/>
+      <c r="D34" s="5">
+        <f t="shared" ref="D34:D65" si="1">PRODUCT(B34,C34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+      <c r="D35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+      <c r="D36" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+      <c r="D38" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="D39" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="D40" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="6"/>
+      <c r="D42" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+      <c r="D43" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="6"/>
+      <c r="D44" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+      <c r="D45" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="D46" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+      <c r="D47" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="6"/>
+      <c r="D48" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="6"/>
+      <c r="D49" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
+      <c r="D50" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="6"/>
+      <c r="D51" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="6"/>
+      <c r="D52" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+      <c r="D53" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="6"/>
+      <c r="D54" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+      <c r="D55" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+      <c r="D56" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="6"/>
+      <c r="D57" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="6"/>
+      <c r="D58" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+      <c r="D59" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+      <c r="D60" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="6"/>
+      <c r="D61" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="4">
-        <f>SUBTOTAL(109,B2:B61)</f>
-        <v>1880</v>
+      <c r="B62" s="4"/>
+      <c r="D62" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🐛 corrigiendo errores visuales en el front
</commit_message>
<xml_diff>
--- a/Documentos/lista de precios.xlsx
+++ b/Documentos/lista de precios.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javja\OneDrive\Escritorio\DomoticMood\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956649B9-8839-4D83-B832-716F1FB0D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4CB8DD-ECDB-4DD3-B917-84E8D211021D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F18A56C-43DA-4260-8C29-14670BEE72CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9F18A56C-43DA-4260-8C29-14670BEE72CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Componente</t>
   </si>
@@ -77,9 +78,6 @@
     <t>Triac</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>Adaptador Smd Tqfp100</t>
   </si>
   <si>
@@ -105,17 +103,139 @@
   </si>
   <si>
     <t>Sensor de lluvia</t>
+  </si>
+  <si>
+    <t>EJERCICIO N°1</t>
+  </si>
+  <si>
+    <t>INVERSION:</t>
+  </si>
+  <si>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>Total Ingresos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>EGRESOS</t>
+  </si>
+  <si>
+    <t>Total Egresos</t>
+  </si>
+  <si>
+    <t>FLUJO DE CAJA ECONÓMICO</t>
+  </si>
+  <si>
+    <t>VA =</t>
+  </si>
+  <si>
+    <t>Inversión=</t>
+  </si>
+  <si>
+    <t>VAN =</t>
+  </si>
+  <si>
+    <t>&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIR = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B/C= </t>
+  </si>
+  <si>
+    <t>B/C=</t>
+  </si>
+  <si>
+    <t>&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Mantenimiento </t>
+  </si>
+  <si>
+    <t>- Predio e impuestos</t>
+  </si>
+  <si>
+    <t>SE DESEA OBTENER UNA RENTABILIDAD DEL 30%</t>
+  </si>
+  <si>
+    <t>- Gastos de producción</t>
+  </si>
+  <si>
+    <t>Mes 0</t>
+  </si>
+  <si>
+    <t>Mes 1</t>
+  </si>
+  <si>
+    <t>Mes 2</t>
+  </si>
+  <si>
+    <t>Mes 3</t>
+  </si>
+  <si>
+    <t>Mes 4</t>
+  </si>
+  <si>
+    <t>Mes 5</t>
+  </si>
+  <si>
+    <t>Mes 6</t>
+  </si>
+  <si>
+    <t>Mes 7</t>
+  </si>
+  <si>
+    <t>Mes 8</t>
+  </si>
+  <si>
+    <t>Mes 9</t>
+  </si>
+  <si>
+    <t>Mes 10</t>
+  </si>
+  <si>
+    <t>Mes 11</t>
+  </si>
+  <si>
+    <t>Mes 12</t>
+  </si>
+  <si>
+    <t>- Cantidad de ventas</t>
+  </si>
+  <si>
+    <t>- Servicio</t>
+  </si>
+  <si>
+    <t>Costo de producto</t>
+  </si>
+  <si>
+    <t>Costo de producción</t>
+  </si>
+  <si>
+    <t>Costo de servicio</t>
+  </si>
+  <si>
+    <t>Costo de mantenimiento</t>
+  </si>
+  <si>
+    <t>&gt;30%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +257,93 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,8 +361,19 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -191,14 +407,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -213,18 +573,63 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="38" fontId="10" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="4"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="38" fontId="12" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="10" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="14" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="12" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="5">
+    <cellStyle name="60% - Énfasis6" xfId="3" builtinId="52"/>
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Salida" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -264,7 +669,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -562,17 +967,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA7C316-E20C-47BC-8E77-A036621AE5C7}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -588,6 +994,12 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="7">
+        <v>6000</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -603,12 +1015,12 @@
         <f t="shared" ref="D2:D33" si="0">PRODUCT(B2,C2)</f>
         <v>440</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>14</v>
+      <c r="F2" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="G2" s="7">
-        <f>SUBTOTAL(109,B2:B61)</f>
-        <v>5685</v>
+        <f>-SUBTOTAL(109,B2:B61)</f>
+        <v>-5685</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,6 +1037,12 @@
         <f t="shared" si="0"/>
         <v>1440</v>
       </c>
+      <c r="F3" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="7">
+        <v>900</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -640,7 +1058,12 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="7">
+        <v>-600</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -734,7 +1157,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <v>385</v>
@@ -749,7 +1172,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <v>385</v>
@@ -764,7 +1187,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <v>790</v>
@@ -779,7 +1202,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <v>300</v>
@@ -794,7 +1217,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <v>350</v>
@@ -809,7 +1232,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2">
         <v>250</v>
@@ -824,7 +1247,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
         <v>180</v>
@@ -839,7 +1262,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>250</v>
@@ -854,7 +1277,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2">
         <v>150</v>
@@ -1182,4 +1605,824 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50A641C-6F75-471C-8BFC-F5BA635CC820}">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="4" max="9" width="14.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="15" width="14.77734375" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15">
+        <f>(D9)*Hoja1!G3</f>
+        <v>900</v>
+      </c>
+      <c r="F8" s="15">
+        <f>SUM(D9:E9)*Hoja1!G3</f>
+        <v>2700</v>
+      </c>
+      <c r="G8" s="15">
+        <f>SUM(D9:F9)*Hoja1!G3</f>
+        <v>5400</v>
+      </c>
+      <c r="H8" s="15">
+        <f>SUM(D9:G9)*Hoja1!G3</f>
+        <v>6300</v>
+      </c>
+      <c r="I8" s="15">
+        <f>SUM(D9:H9)*Hoja1!G3</f>
+        <v>8100</v>
+      </c>
+      <c r="J8" s="15">
+        <f>SUM(D9:I9)*Hoja1!G3</f>
+        <v>9000</v>
+      </c>
+      <c r="K8" s="15">
+        <f>SUM(D9:J9)*Hoja1!G3</f>
+        <v>10800</v>
+      </c>
+      <c r="L8" s="15">
+        <f>SUM(D9:K9)*Hoja1!G3</f>
+        <v>11700</v>
+      </c>
+      <c r="M8" s="15">
+        <f>SUM(D9:L9)*Hoja1!G3</f>
+        <v>18900</v>
+      </c>
+      <c r="N8" s="15">
+        <f>SUM(D9:M9)*Hoja1!G3</f>
+        <v>19800</v>
+      </c>
+      <c r="O8" s="15">
+        <f>SUM(D9:N9)*Hoja1!G3</f>
+        <v>21600</v>
+      </c>
+      <c r="P8" s="15">
+        <f>SUM(D9:O9)*Hoja1!G3</f>
+        <v>24300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>2</v>
+      </c>
+      <c r="F9" s="15">
+        <v>3</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1</v>
+      </c>
+      <c r="J9" s="15">
+        <v>2</v>
+      </c>
+      <c r="K9" s="15">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <v>8</v>
+      </c>
+      <c r="M9" s="15">
+        <v>1</v>
+      </c>
+      <c r="N9" s="15">
+        <v>2</v>
+      </c>
+      <c r="O9" s="15">
+        <v>3</v>
+      </c>
+      <c r="P9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="19">
+        <f>SUM(D7:D9)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="19">
+        <f>Hoja1!G1*Hoja2!E9+Hoja2!E8</f>
+        <v>12900</v>
+      </c>
+      <c r="F10" s="19">
+        <f>Hoja1!G1*Hoja2!F9+Hoja2!F8</f>
+        <v>20700</v>
+      </c>
+      <c r="G10" s="19">
+        <f>Hoja1!G1*Hoja2!G9+Hoja2!G8</f>
+        <v>11400</v>
+      </c>
+      <c r="H10" s="19">
+        <f>Hoja1!G1*Hoja2!H9+Hoja2!H8</f>
+        <v>18300</v>
+      </c>
+      <c r="I10" s="19">
+        <f>Hoja1!G1*Hoja2!I9+Hoja2!I8</f>
+        <v>14100</v>
+      </c>
+      <c r="J10" s="19">
+        <f>Hoja1!G1*Hoja2!J9+Hoja2!J8</f>
+        <v>21000</v>
+      </c>
+      <c r="K10" s="19">
+        <f>Hoja1!G1*Hoja2!K9+Hoja2!K8</f>
+        <v>16800</v>
+      </c>
+      <c r="L10" s="19">
+        <f>Hoja1!G1*Hoja2!L9+Hoja2!L8</f>
+        <v>59700</v>
+      </c>
+      <c r="M10" s="19">
+        <f>Hoja1!G1*Hoja2!M9+Hoja2!M8</f>
+        <v>24900</v>
+      </c>
+      <c r="N10" s="19">
+        <f>Hoja1!G1*Hoja2!N9+Hoja2!N8</f>
+        <v>31800</v>
+      </c>
+      <c r="O10" s="19">
+        <f>Hoja1!G1*Hoja2!O9+Hoja2!O8</f>
+        <v>39600</v>
+      </c>
+      <c r="P10" s="19">
+        <f>Hoja1!G1*Hoja2!P9+Hoja2!P8</f>
+        <v>30300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="42">
+        <f>Hoja1!G2*D9</f>
+        <v>-5685</v>
+      </c>
+      <c r="E13" s="42">
+        <f>Hoja1!G2*E9</f>
+        <v>-11370</v>
+      </c>
+      <c r="F13" s="42">
+        <f>Hoja1!G2*F9</f>
+        <v>-17055</v>
+      </c>
+      <c r="G13" s="42">
+        <f>Hoja1!G2*G9</f>
+        <v>-5685</v>
+      </c>
+      <c r="H13" s="42">
+        <f>Hoja1!G2*H9</f>
+        <v>-11370</v>
+      </c>
+      <c r="I13" s="42">
+        <f>Hoja1!G2*I9</f>
+        <v>-5685</v>
+      </c>
+      <c r="J13" s="42">
+        <f>Hoja1!G2*J9</f>
+        <v>-11370</v>
+      </c>
+      <c r="K13" s="42">
+        <f>Hoja1!G2*K9</f>
+        <v>-5685</v>
+      </c>
+      <c r="L13" s="42">
+        <f>Hoja1!G2*L9</f>
+        <v>-45480</v>
+      </c>
+      <c r="M13" s="42">
+        <f>Hoja1!G2*M9</f>
+        <v>-5685</v>
+      </c>
+      <c r="N13" s="42">
+        <f>Hoja1!G2*N9</f>
+        <v>-11370</v>
+      </c>
+      <c r="O13" s="42">
+        <f>Hoja1!G2*O9</f>
+        <v>-17055</v>
+      </c>
+      <c r="P13" s="42">
+        <f>Hoja1!G2*P9</f>
+        <v>-5685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="E14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="F14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="G14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="H14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="I14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="J14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="K14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="L14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="M14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="N14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="O14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+      <c r="P14" s="42">
+        <f>Hoja1!G4</f>
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="F15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="G15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="H15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="I15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="J15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="K15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="L15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="M15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="N15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="O15" s="43">
+        <v>-200</v>
+      </c>
+      <c r="P15" s="43">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="43">
+        <f>SUM(D13:D15)</f>
+        <v>-6285</v>
+      </c>
+      <c r="E16" s="43">
+        <f t="shared" ref="E16:F16" si="0">SUM(E13:E15)</f>
+        <v>-12170</v>
+      </c>
+      <c r="F16" s="43">
+        <f t="shared" si="0"/>
+        <v>-17855</v>
+      </c>
+      <c r="G16" s="43">
+        <f t="shared" ref="G16:O16" si="1">SUM(G13:G15)</f>
+        <v>-6485</v>
+      </c>
+      <c r="H16" s="43">
+        <f t="shared" si="1"/>
+        <v>-12170</v>
+      </c>
+      <c r="I16" s="43">
+        <f t="shared" si="1"/>
+        <v>-6485</v>
+      </c>
+      <c r="J16" s="43">
+        <f t="shared" si="1"/>
+        <v>-12170</v>
+      </c>
+      <c r="K16" s="43">
+        <f t="shared" si="1"/>
+        <v>-6485</v>
+      </c>
+      <c r="L16" s="43">
+        <f t="shared" si="1"/>
+        <v>-46280</v>
+      </c>
+      <c r="M16" s="43">
+        <f t="shared" si="1"/>
+        <v>-6485</v>
+      </c>
+      <c r="N16" s="43">
+        <f t="shared" si="1"/>
+        <v>-12170</v>
+      </c>
+      <c r="O16" s="43">
+        <f t="shared" si="1"/>
+        <v>-17855</v>
+      </c>
+      <c r="P16" s="43">
+        <f>SUM(P13:P15)</f>
+        <v>-6485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="41">
+        <f>SUM(D10,D16)</f>
+        <v>-6284</v>
+      </c>
+      <c r="E18" s="41">
+        <f t="shared" ref="E18:F18" si="2">SUM(E10,E16)</f>
+        <v>730</v>
+      </c>
+      <c r="F18" s="41">
+        <f t="shared" si="2"/>
+        <v>2845</v>
+      </c>
+      <c r="G18" s="41">
+        <f t="shared" ref="G18:O18" si="3">SUM(G10,G16)</f>
+        <v>4915</v>
+      </c>
+      <c r="H18" s="41">
+        <f t="shared" si="3"/>
+        <v>6130</v>
+      </c>
+      <c r="I18" s="41">
+        <f t="shared" si="3"/>
+        <v>7615</v>
+      </c>
+      <c r="J18" s="41">
+        <f t="shared" si="3"/>
+        <v>8830</v>
+      </c>
+      <c r="K18" s="41">
+        <f t="shared" si="3"/>
+        <v>10315</v>
+      </c>
+      <c r="L18" s="41">
+        <f t="shared" si="3"/>
+        <v>13420</v>
+      </c>
+      <c r="M18" s="41">
+        <f t="shared" si="3"/>
+        <v>18415</v>
+      </c>
+      <c r="N18" s="41">
+        <f t="shared" si="3"/>
+        <v>19630</v>
+      </c>
+      <c r="O18" s="41">
+        <f t="shared" si="3"/>
+        <v>21745</v>
+      </c>
+      <c r="P18" s="41">
+        <f>SUM(P10,P16)</f>
+        <v>23815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="30">
+        <f>NPV(30%,D18:P18)</f>
+        <v>9930.5342394431027</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="31">
+        <f>D13</f>
+        <v>-5685</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="32">
+        <f>SUM(C20:C21)</f>
+        <v>4245.5342394431027</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="33">
+        <f>IRR(D18:P18)</f>
+        <v>0.60128431065643917</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="30">
+        <f>C20</f>
+        <v>9930.5342394431027</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="9"/>
+      <c r="C27" s="34">
+        <f>-C21</f>
+        <v>5685</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="35">
+        <f>C26/C27</f>
+        <v>1.7467958204825158</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>